<commit_message>
Excel ML Log Writer works
</commit_message>
<xml_diff>
--- a/excel_manipulation/Logs.xlsx
+++ b/excel_manipulation/Logs.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:I6"/>
+  <dimension ref="A3:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,6 +582,90 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BINARY</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>24:48:1024</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-03-04</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1024</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BINARY</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>24:48:1024</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-03-09</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1024</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BINARY</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>24:48:1024</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-04-34</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1024</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -594,7 +678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:M6"/>
+  <dimension ref="A3:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -816,6 +900,138 @@
         <v>0.9099</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BINARY</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>24:48:1024</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-03-04</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1024</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-03-04</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>DEF.txt</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.9099</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BINARY</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>24:48:1024</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-03-09</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1024</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-03-09</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>DEF.txt</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.9099</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BINARY</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>24:48:1024</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-04-34</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1024</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2021-09-06-23-04-34</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>DEF.txt</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.9099</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>